<commit_message>
adding checks for tasmin
</commit_message>
<xml_diff>
--- a/LOCA2_inventory_min_errors.xlsx
+++ b/LOCA2_inventory_min_errors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wjc/GitHub/LOCA2_Prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148A600E-8E2B-C047-8FD1-93283E11FB20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A6C103-A658-4248-9876-31642A336087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10360" yWindow="500" windowWidth="28040" windowHeight="17780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1027,7 +1027,7 @@
   <dimension ref="A1:G676"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D476" sqref="D476"/>
+      <selection activeCell="A651" sqref="A651:XFD651"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9085,26 +9085,26 @@
         <v>2.4186773239999999</v>
       </c>
     </row>
-    <row r="351" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A351" t="s">
+    <row r="351" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A351" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B351" t="s">
+      <c r="B351" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C351" t="s">
+      <c r="C351" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D351" t="s">
+      <c r="D351" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E351">
+      <c r="E351" s="1">
         <v>9.8579916819999998</v>
       </c>
-      <c r="F351">
+      <c r="F351" s="1">
         <v>1.2</v>
       </c>
-      <c r="G351">
+      <c r="G351" s="1">
         <v>9.9307602930000005</v>
       </c>
     </row>
@@ -13686,25 +13686,25 @@
       </c>
     </row>
     <row r="551" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A551" t="s">
+      <c r="A551" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B551" t="s">
+      <c r="B551" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C551" t="s">
+      <c r="C551" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D551" t="s">
+      <c r="D551" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E551">
+      <c r="E551" s="1">
         <v>10.55698821</v>
       </c>
-      <c r="F551">
+      <c r="F551" s="1">
         <v>2.7166155409999999</v>
       </c>
-      <c r="G551">
+      <c r="G551" s="1">
         <v>10.90091739</v>
       </c>
     </row>
@@ -15985,26 +15985,26 @@
         <v>5.6824290580000003</v>
       </c>
     </row>
-    <row r="651" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A651" t="s">
+    <row r="651" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A651" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B651" t="s">
+      <c r="B651" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C651" t="s">
+      <c r="C651" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D651" t="s">
+      <c r="D651" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E651">
+      <c r="E651" s="1">
         <v>11.868024269999999</v>
       </c>
-      <c r="F651">
+      <c r="F651" s="1">
         <v>1.403566885</v>
       </c>
-      <c r="G651">
+      <c r="G651" s="1">
         <v>11.950732199999999</v>
       </c>
     </row>

</xml_diff>